<commit_message>
Update meter import tools to accept current ESPM  format
</commit_message>
<xml_diff>
--- a/seed/data_importer/tests/data/example-pm-monthly-meter-usage-1-dup.xlsx
+++ b/seed/data_importer/tests/data/example-pm-monthly-meter-usage-1-dup.xlsx
@@ -1,67 +1,188 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr date1904="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Meter Entries" sheetId="1" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
-  <si>
-    <t>example-monthly-metrics</t>
-  </si>
-  <si>
-    <t>Data Request:Monthly Metrics</t>
-  </si>
-  <si>
-    <t>Date Downloaded: 08/28/2018 10:29 AM EDT</t>
-  </si>
-  <si>
-    <t>Date Generated: 08/28/2018 10:29 AM EDT</t>
-  </si>
-  <si>
-    <t>Property Id</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="57">
+  <si>
+    <t>My Portfolio: Test City SEED</t>
+  </si>
+  <si>
+    <t>06/06/2019 04:28 PM EDT</t>
+  </si>
+  <si>
+    <t>Total Properties: 1</t>
+  </si>
+  <si>
+    <t>Additional Information for Electric Meters with Green Power</t>
+  </si>
+  <si>
+    <t>Additional Information for On-Site Renewable Meters</t>
+  </si>
+  <si>
+    <t>Additional Information for Disposed Waste Meters</t>
   </si>
   <si>
     <t>Property Name</t>
   </si>
   <si>
-    <t>Parent Property Id</t>
-  </si>
-  <si>
-    <t>Parent Property Name</t>
-  </si>
-  <si>
-    <t>Month</t>
-  </si>
-  <si>
-    <t>Electricity Use  (kBtu)</t>
-  </si>
-  <si>
-    <t>Natural Gas Use  (kBtu)</t>
-  </si>
-  <si>
-    <t>EPA Sample Library</t>
-  </si>
-  <si>
-    <t>Not Applicable: Standalone Property</t>
-  </si>
-  <si>
-    <t>Jan-16</t>
-  </si>
-  <si>
-    <t>Feb-16</t>
-  </si>
-  <si>
-    <t>EPA Sample K-12 School</t>
-  </si>
-  <si>
-    <t>Mar-16</t>
+    <t>Portfolio Manager ID</t>
+  </si>
+  <si>
+    <t>Portfolio Manager Meter ID</t>
+  </si>
+  <si>
+    <t>Meter Name</t>
+  </si>
+  <si>
+    <t>Meter Type</t>
+  </si>
+  <si>
+    <t>Meter Consumption ID</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>Delivery Date</t>
+  </si>
+  <si>
+    <t>Usage/Quantity</t>
+  </si>
+  <si>
+    <t>Usage Units</t>
+  </si>
+  <si>
+    <t>Cost ($)</t>
+  </si>
+  <si>
+    <t>Estimation?</t>
+  </si>
+  <si>
+    <t>Demand (kW)</t>
+  </si>
+  <si>
+    <t>Demand Cost ($)</t>
+  </si>
+  <si>
+    <t>Last Modified Date</t>
+  </si>
+  <si>
+    <t>Last Modified By</t>
+  </si>
+  <si>
+    <t>Green Power</t>
+  </si>
+  <si>
+    <t>Green Power Quantity</t>
+  </si>
+  <si>
+    <t>Fuel Source -Biogas %</t>
+  </si>
+  <si>
+    <t>Fuel Source -Biomass %</t>
+  </si>
+  <si>
+    <t>Fuel Source - Geothermal %</t>
+  </si>
+  <si>
+    <t>Fuel Source - Small Hydropower %</t>
+  </si>
+  <si>
+    <t>Fuel Source - Solar %</t>
+  </si>
+  <si>
+    <t>Fuel Souce - Wind %</t>
+  </si>
+  <si>
+    <t>Fuel Source - Unknown %</t>
+  </si>
+  <si>
+    <t>Green Power Generation Location</t>
+  </si>
+  <si>
+    <t>Generation Facility ID</t>
+  </si>
+  <si>
+    <t>Generation Facility Name</t>
+  </si>
+  <si>
+    <t>eGRID Subregion or Province</t>
+  </si>
+  <si>
+    <t>On-Site Renewable System Energy Used On-Site</t>
+  </si>
+  <si>
+    <t>Onsite Renewable System Energy Used Onsite Units</t>
+  </si>
+  <si>
+    <t>Onsite Renewable System Energy Exported Offsite</t>
+  </si>
+  <si>
+    <t>Onsite Renewable System Energy Exported Offsite Units</t>
+  </si>
+  <si>
+    <t>REC Ownership</t>
+  </si>
+  <si>
+    <t>Disposed Waste - Landfill %</t>
+  </si>
+  <si>
+    <t>Disposed Waste - Incineration %</t>
+  </si>
+  <si>
+    <t>Disposed Waste - Waste to Energy %</t>
+  </si>
+  <si>
+    <t>Disposed Waste - Don't Know %</t>
+  </si>
+  <si>
+    <t>Campus Building 1</t>
+  </si>
+  <si>
+    <t>5766973-0</t>
+  </si>
+  <si>
+    <t>Electric Grid Meter</t>
+  </si>
+  <si>
+    <t>Electric - Grid</t>
+  </si>
+  <si>
+    <t>Not Available</t>
+  </si>
+  <si>
+    <t>kBtu (thousand Btu)</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>SEED_Owner_Test</t>
+  </si>
+  <si>
+    <t>5766975-0</t>
+  </si>
+  <si>
+    <t>5766973-1</t>
+  </si>
+  <si>
+    <t>Natural Gas</t>
+  </si>
+  <si>
+    <t>5766975-1</t>
   </si>
 </sst>
 </file>
@@ -72,7 +193,7 @@
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="59" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -89,13 +210,27 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <b val="1"/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color indexed="8"/>
-      <name val="Helvetica Neue"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -110,7 +245,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor indexed="11"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor indexed="12"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -120,8 +267,20 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="15"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="16"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -133,23 +292,64 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
       <right/>
       <top style="thin">
         <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="11"/>
+        <color indexed="8"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
+      <top/>
       <bottom style="thin">
-        <color indexed="11"/>
+        <color indexed="8"/>
       </bottom>
       <diagonal/>
     </border>
@@ -162,112 +362,22 @@
         <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="11"/>
+        <color indexed="8"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="11"/>
+        <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="11"/>
+        <color indexed="8"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
+        <color indexed="8"/>
       </bottom>
       <diagonal/>
     </border>
@@ -277,63 +387,69 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
+    <xf numFmtId="49" fontId="6" fillId="7" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
+    <xf numFmtId="49" fontId="6" fillId="8" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="59" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
+    <xf numFmtId="59" fontId="5" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -354,10 +470,12 @@
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ff8fc76f"/>
+      <rgbColor rgb="ff87b2dc"/>
+      <rgbColor rgb="ffebb57e"/>
+      <rgbColor rgb="ffeaf7e3"/>
+      <rgbColor rgb="ffd4e6f6"/>
+      <rgbColor rgb="ffffebd8"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1422,22 +1540,17 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:AM18"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.33333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="36.8516" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.3516" style="1" customWidth="1"/>
-    <col min="3" max="4" width="28.6719" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.85156" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.3516" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19" style="1" customWidth="1"/>
-    <col min="8" max="256" width="8.35156" style="1" customWidth="1"/>
+    <col min="1" max="39" width="20" style="1" customWidth="1"/>
+    <col min="40" max="256" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.65" customHeight="1">
+    <row r="1" ht="17" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
@@ -1446,217 +1559,1769 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
-      <c r="G1" s="4"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="3"/>
+      <c r="AC1" s="3"/>
+      <c r="AD1" s="3"/>
+      <c r="AE1" s="3"/>
+      <c r="AF1" s="3"/>
+      <c r="AG1" s="3"/>
+      <c r="AH1" s="3"/>
+      <c r="AI1" s="3"/>
+      <c r="AJ1" s="3"/>
+      <c r="AK1" s="3"/>
+      <c r="AL1" s="3"/>
+      <c r="AM1" s="3"/>
     </row>
-    <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="5">
+    <row r="2" ht="15" customHeight="1">
+      <c r="A2" t="s" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+      <c r="AC2" s="3"/>
+      <c r="AD2" s="3"/>
+      <c r="AE2" s="3"/>
+      <c r="AF2" s="3"/>
+      <c r="AG2" s="3"/>
+      <c r="AH2" s="3"/>
+      <c r="AI2" s="3"/>
+      <c r="AJ2" s="3"/>
+      <c r="AK2" s="3"/>
+      <c r="AL2" s="3"/>
+      <c r="AM2" s="3"/>
     </row>
-    <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" t="s" s="7">
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" t="s" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="3"/>
+      <c r="AE3" s="3"/>
+      <c r="AF3" s="3"/>
+      <c r="AG3" s="3"/>
+      <c r="AH3" s="3"/>
+      <c r="AI3" s="3"/>
+      <c r="AJ3" s="3"/>
+      <c r="AK3" s="3"/>
+      <c r="AL3" s="3"/>
+      <c r="AM3" s="3"/>
     </row>
-    <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="10">
+    <row r="4" ht="15" customHeight="1">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+      <c r="AC4" s="3"/>
+      <c r="AD4" s="3"/>
+      <c r="AE4" s="5"/>
+      <c r="AF4" s="3"/>
+      <c r="AG4" s="3"/>
+      <c r="AH4" s="3"/>
+      <c r="AI4" s="3"/>
+      <c r="AJ4" s="5"/>
+      <c r="AK4" s="3"/>
+      <c r="AL4" s="3"/>
+      <c r="AM4" s="3"/>
+    </row>
+    <row r="5" ht="15" customHeight="1">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" t="s" s="8">
         <v>3</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="6"/>
+      <c r="AA5" s="6"/>
+      <c r="AB5" s="6"/>
+      <c r="AC5" s="6"/>
+      <c r="AD5" s="7"/>
+      <c r="AE5" t="s" s="10">
+        <v>4</v>
+      </c>
+      <c r="AF5" s="9"/>
+      <c r="AG5" s="6"/>
+      <c r="AH5" s="6"/>
+      <c r="AI5" s="7"/>
+      <c r="AJ5" t="s" s="11">
+        <v>5</v>
+      </c>
+      <c r="AK5" s="9"/>
+      <c r="AL5" s="6"/>
+      <c r="AM5" s="6"/>
     </row>
-    <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="13"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
+    <row r="6" ht="60" customHeight="1">
+      <c r="A6" t="s" s="12">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s" s="12">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s" s="12">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s" s="12">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s" s="12">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s" s="12">
+        <v>11</v>
+      </c>
+      <c r="G6" t="s" s="12">
+        <v>12</v>
+      </c>
+      <c r="H6" t="s" s="12">
+        <v>13</v>
+      </c>
+      <c r="I6" t="s" s="12">
+        <v>14</v>
+      </c>
+      <c r="J6" t="s" s="12">
+        <v>15</v>
+      </c>
+      <c r="K6" t="s" s="12">
+        <v>16</v>
+      </c>
+      <c r="L6" t="s" s="12">
+        <v>17</v>
+      </c>
+      <c r="M6" t="s" s="12">
+        <v>18</v>
+      </c>
+      <c r="N6" t="s" s="12">
+        <v>19</v>
+      </c>
+      <c r="O6" t="s" s="12">
+        <v>20</v>
+      </c>
+      <c r="P6" t="s" s="12">
+        <v>21</v>
+      </c>
+      <c r="Q6" t="s" s="12">
+        <v>22</v>
+      </c>
+      <c r="R6" t="s" s="13">
+        <v>23</v>
+      </c>
+      <c r="S6" t="s" s="13">
+        <v>24</v>
+      </c>
+      <c r="T6" t="s" s="13">
+        <v>25</v>
+      </c>
+      <c r="U6" t="s" s="13">
+        <v>26</v>
+      </c>
+      <c r="V6" t="s" s="13">
+        <v>27</v>
+      </c>
+      <c r="W6" t="s" s="13">
+        <v>28</v>
+      </c>
+      <c r="X6" t="s" s="13">
+        <v>29</v>
+      </c>
+      <c r="Y6" t="s" s="13">
+        <v>30</v>
+      </c>
+      <c r="Z6" t="s" s="13">
+        <v>31</v>
+      </c>
+      <c r="AA6" t="s" s="13">
+        <v>32</v>
+      </c>
+      <c r="AB6" t="s" s="13">
+        <v>33</v>
+      </c>
+      <c r="AC6" t="s" s="13">
+        <v>34</v>
+      </c>
+      <c r="AD6" t="s" s="13">
+        <v>35</v>
+      </c>
+      <c r="AE6" t="s" s="14">
+        <v>36</v>
+      </c>
+      <c r="AF6" t="s" s="14">
+        <v>37</v>
+      </c>
+      <c r="AG6" t="s" s="14">
+        <v>38</v>
+      </c>
+      <c r="AH6" t="s" s="14">
+        <v>39</v>
+      </c>
+      <c r="AI6" t="s" s="14">
+        <v>40</v>
+      </c>
+      <c r="AJ6" t="s" s="15">
+        <v>41</v>
+      </c>
+      <c r="AK6" t="s" s="15">
+        <v>42</v>
+      </c>
+      <c r="AL6" t="s" s="15">
+        <v>43</v>
+      </c>
+      <c r="AM6" t="s" s="15">
+        <v>44</v>
+      </c>
     </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" t="s" s="10">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s" s="14">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s" s="15">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s" s="15">
-        <v>7</v>
-      </c>
-      <c r="E6" t="s" s="15">
-        <v>8</v>
-      </c>
-      <c r="F6" t="s" s="15">
-        <v>9</v>
-      </c>
-      <c r="G6" t="s" s="15">
-        <v>10</v>
+    <row r="7" ht="30" customHeight="1">
+      <c r="A7" t="s" s="16">
+        <v>45</v>
+      </c>
+      <c r="B7" s="17">
+        <v>5766973</v>
+      </c>
+      <c r="C7" t="s" s="18">
+        <v>46</v>
+      </c>
+      <c r="D7" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E7" t="s" s="16">
+        <v>48</v>
+      </c>
+      <c r="F7" s="17">
+        <v>809588892</v>
+      </c>
+      <c r="G7" s="19">
+        <v>40908</v>
+      </c>
+      <c r="H7" s="19">
+        <v>40939</v>
+      </c>
+      <c r="I7" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="J7" s="20">
+        <v>597478.9</v>
+      </c>
+      <c r="K7" t="s" s="16">
+        <v>50</v>
+      </c>
+      <c r="L7" s="17">
+        <v>4342</v>
+      </c>
+      <c r="M7" t="s" s="16">
+        <v>51</v>
+      </c>
+      <c r="N7" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="O7" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="P7" s="19">
+        <v>42159</v>
+      </c>
+      <c r="Q7" t="s" s="16">
+        <v>52</v>
+      </c>
+      <c r="R7" t="s" s="16">
+        <v>51</v>
+      </c>
+      <c r="S7" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="T7" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="U7" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="V7" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="W7" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="X7" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="Y7" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="Z7" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AA7" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AB7" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AC7" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AD7" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AE7" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AF7" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AG7" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AH7" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AI7" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AJ7" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AK7" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AL7" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AM7" t="s" s="16">
+        <v>49</v>
       </c>
     </row>
-    <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="16">
+    <row r="8" ht="30" customHeight="1">
+      <c r="A8" t="s" s="16">
+        <v>45</v>
+      </c>
+      <c r="B8" s="17">
         <v>5766973</v>
       </c>
-      <c r="B7" t="s" s="14">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s" s="15">
-        <v>12</v>
-      </c>
-      <c r="D7" t="s" s="15">
-        <v>12</v>
-      </c>
-      <c r="E7" t="s" s="15">
-        <v>13</v>
-      </c>
-      <c r="F7" s="17">
-        <v>597478.9</v>
-      </c>
-      <c r="G7" s="17">
+      <c r="C8" t="s" s="18">
+        <v>46</v>
+      </c>
+      <c r="D8" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E8" t="s" s="16">
+        <v>48</v>
+      </c>
+      <c r="F8" s="17">
+        <v>809589378</v>
+      </c>
+      <c r="G8" s="19">
+        <v>40939</v>
+      </c>
+      <c r="H8" s="19">
+        <v>40968</v>
+      </c>
+      <c r="I8" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="J8" s="20">
+        <v>548603.7</v>
+      </c>
+      <c r="K8" t="s" s="16">
+        <v>50</v>
+      </c>
+      <c r="L8" s="17">
+        <v>4975.55</v>
+      </c>
+      <c r="M8" t="s" s="16">
+        <v>51</v>
+      </c>
+      <c r="N8" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="O8" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="P8" s="19">
+        <v>42159</v>
+      </c>
+      <c r="Q8" t="s" s="16">
+        <v>52</v>
+      </c>
+      <c r="R8" t="s" s="16">
+        <v>51</v>
+      </c>
+      <c r="S8" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="T8" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="U8" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="V8" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="W8" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="X8" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="Y8" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="Z8" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AA8" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AB8" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AC8" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AD8" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AE8" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AF8" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AG8" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AH8" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AI8" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AJ8" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AK8" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AL8" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AM8" t="s" s="16">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" ht="30" customHeight="1">
+      <c r="A9" t="s" s="16">
+        <v>45</v>
+      </c>
+      <c r="B9" s="17">
+        <v>5766975</v>
+      </c>
+      <c r="C9" t="s" s="18">
+        <v>53</v>
+      </c>
+      <c r="D9" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E9" t="s" s="16">
+        <v>48</v>
+      </c>
+      <c r="F9" s="17">
+        <v>2938212691</v>
+      </c>
+      <c r="G9" s="19">
+        <v>40908</v>
+      </c>
+      <c r="H9" s="19">
+        <v>40939</v>
+      </c>
+      <c r="I9" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="J9" s="20">
+        <v>154572.2</v>
+      </c>
+      <c r="K9" t="s" s="16">
+        <v>50</v>
+      </c>
+      <c r="L9" s="17">
+        <v>4915</v>
+      </c>
+      <c r="M9" t="s" s="16">
+        <v>51</v>
+      </c>
+      <c r="N9" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="O9" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="P9" s="19">
+        <v>42159</v>
+      </c>
+      <c r="Q9" t="s" s="16">
+        <v>52</v>
+      </c>
+      <c r="R9" t="s" s="16">
+        <v>51</v>
+      </c>
+      <c r="S9" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="T9" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="U9" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="V9" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="W9" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="X9" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="Y9" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="Z9" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AA9" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AB9" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AC9" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AD9" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AE9" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AF9" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AG9" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AH9" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AI9" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AJ9" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AK9" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AL9" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AM9" t="s" s="16">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" ht="30" customHeight="1">
+      <c r="A10" t="s" s="16">
+        <v>45</v>
+      </c>
+      <c r="B10" s="17">
+        <v>5766975</v>
+      </c>
+      <c r="C10" t="s" s="18">
+        <v>53</v>
+      </c>
+      <c r="D10" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E10" t="s" s="16">
+        <v>48</v>
+      </c>
+      <c r="F10" s="17">
+        <v>2938212692</v>
+      </c>
+      <c r="G10" s="19">
+        <v>40939</v>
+      </c>
+      <c r="H10" s="19">
+        <v>40968</v>
+      </c>
+      <c r="I10" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="J10" s="20">
+        <v>141437.5</v>
+      </c>
+      <c r="K10" t="s" s="16">
+        <v>50</v>
+      </c>
+      <c r="L10" s="17">
+        <v>4180</v>
+      </c>
+      <c r="M10" t="s" s="16">
+        <v>51</v>
+      </c>
+      <c r="N10" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="O10" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="P10" s="19">
+        <v>42159</v>
+      </c>
+      <c r="Q10" t="s" s="16">
+        <v>52</v>
+      </c>
+      <c r="R10" t="s" s="16">
+        <v>51</v>
+      </c>
+      <c r="S10" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="T10" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="U10" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="V10" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="W10" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="X10" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="Y10" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="Z10" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AA10" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AB10" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AC10" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AD10" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AE10" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AF10" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AG10" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AH10" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AI10" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AJ10" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AK10" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AL10" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AM10" t="s" s="16">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" ht="30" customHeight="1">
+      <c r="A11" t="s" s="16">
+        <v>45</v>
+      </c>
+      <c r="B11" s="17">
+        <v>5766973</v>
+      </c>
+      <c r="C11" t="s" s="18">
+        <v>54</v>
+      </c>
+      <c r="D11" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E11" t="s" s="16">
+        <v>55</v>
+      </c>
+      <c r="F11" s="17">
+        <v>2938212693</v>
+      </c>
+      <c r="G11" s="19">
+        <v>40908</v>
+      </c>
+      <c r="H11" s="19">
+        <v>40939</v>
+      </c>
+      <c r="I11" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="J11" s="20">
         <v>576000.2</v>
       </c>
+      <c r="K11" t="s" s="16">
+        <v>50</v>
+      </c>
+      <c r="L11" s="17">
+        <v>4020.24</v>
+      </c>
+      <c r="M11" t="s" s="16">
+        <v>51</v>
+      </c>
+      <c r="N11" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="O11" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="P11" s="19">
+        <v>42159</v>
+      </c>
+      <c r="Q11" t="s" s="16">
+        <v>52</v>
+      </c>
+      <c r="R11" t="s" s="16">
+        <v>51</v>
+      </c>
+      <c r="S11" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="T11" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="U11" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="V11" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="W11" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="X11" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="Y11" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="Z11" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AA11" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AB11" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AC11" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AD11" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AE11" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AF11" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AG11" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AH11" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AI11" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AJ11" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AK11" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AL11" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AM11" t="s" s="16">
+        <v>49</v>
+      </c>
     </row>
-    <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="16">
+    <row r="12" ht="30" customHeight="1">
+      <c r="A12" t="s" s="16">
+        <v>45</v>
+      </c>
+      <c r="B12" s="17">
         <v>5766973</v>
       </c>
-      <c r="B8" t="s" s="14">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s" s="15">
-        <v>12</v>
-      </c>
-      <c r="D8" t="s" s="15">
-        <v>12</v>
-      </c>
-      <c r="E8" t="s" s="15">
-        <v>14</v>
-      </c>
-      <c r="F8" s="17">
-        <v>548603.7</v>
-      </c>
-      <c r="G8" s="17">
+      <c r="C12" t="s" s="18">
+        <v>54</v>
+      </c>
+      <c r="D12" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E12" t="s" s="16">
+        <v>55</v>
+      </c>
+      <c r="F12" s="17">
+        <v>2938212694</v>
+      </c>
+      <c r="G12" s="19">
+        <v>40939</v>
+      </c>
+      <c r="H12" s="19">
+        <v>40968</v>
+      </c>
+      <c r="I12" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="J12" s="20">
         <v>488000.1</v>
       </c>
+      <c r="K12" t="s" s="16">
+        <v>50</v>
+      </c>
+      <c r="L12" s="17">
+        <v>3859.62</v>
+      </c>
+      <c r="M12" t="s" s="16">
+        <v>51</v>
+      </c>
+      <c r="N12" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="O12" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="P12" s="19">
+        <v>42159</v>
+      </c>
+      <c r="Q12" t="s" s="16">
+        <v>52</v>
+      </c>
+      <c r="R12" t="s" s="16">
+        <v>51</v>
+      </c>
+      <c r="S12" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="T12" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="U12" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="V12" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="W12" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="X12" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="Y12" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="Z12" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AA12" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AB12" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AC12" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AD12" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AE12" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AF12" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AG12" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AH12" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AI12" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AJ12" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AK12" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AL12" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AM12" t="s" s="16">
+        <v>49</v>
+      </c>
     </row>
-    <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="16">
+    <row r="13" ht="30" customHeight="1">
+      <c r="A13" t="s" s="16">
+        <v>45</v>
+      </c>
+      <c r="B13" s="17">
         <v>5766975</v>
       </c>
-      <c r="B9" t="s" s="14">
-        <v>15</v>
-      </c>
-      <c r="C9" t="s" s="15">
-        <v>12</v>
-      </c>
-      <c r="D9" t="s" s="15">
-        <v>12</v>
-      </c>
-      <c r="E9" t="s" s="15">
-        <v>13</v>
-      </c>
-      <c r="F9" s="17">
-        <v>154572.2</v>
-      </c>
-      <c r="G9" s="18">
+      <c r="C13" t="s" s="18">
+        <v>56</v>
+      </c>
+      <c r="D13" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E13" t="s" s="16">
+        <v>55</v>
+      </c>
+      <c r="F13" s="17">
+        <v>2938212695</v>
+      </c>
+      <c r="G13" s="19">
+        <v>40908</v>
+      </c>
+      <c r="H13" s="19">
+        <v>40939</v>
+      </c>
+      <c r="I13" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="J13" s="17">
         <v>299915</v>
       </c>
+      <c r="K13" t="s" s="16">
+        <v>50</v>
+      </c>
+      <c r="L13" s="17">
+        <v>4296</v>
+      </c>
+      <c r="M13" t="s" s="16">
+        <v>51</v>
+      </c>
+      <c r="N13" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="O13" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="P13" s="19">
+        <v>42159</v>
+      </c>
+      <c r="Q13" t="s" s="16">
+        <v>52</v>
+      </c>
+      <c r="R13" t="s" s="16">
+        <v>51</v>
+      </c>
+      <c r="S13" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="T13" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="U13" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="V13" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="W13" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="X13" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="Y13" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="Z13" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AA13" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AB13" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AC13" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AD13" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AE13" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AF13" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AG13" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AH13" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AI13" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AJ13" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AK13" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AL13" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AM13" t="s" s="16">
+        <v>49</v>
+      </c>
     </row>
-    <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="16">
+    <row r="14" ht="30" customHeight="1">
+      <c r="A14" t="s" s="16">
+        <v>45</v>
+      </c>
+      <c r="B14" s="17">
         <v>5766975</v>
       </c>
-      <c r="B10" t="s" s="14">
-        <v>15</v>
-      </c>
-      <c r="C10" t="s" s="15">
-        <v>12</v>
-      </c>
-      <c r="D10" t="s" s="15">
-        <v>12</v>
-      </c>
-      <c r="E10" t="s" s="15">
-        <v>14</v>
-      </c>
-      <c r="F10" s="17">
-        <v>141437.5</v>
-      </c>
-      <c r="G10" s="17">
+      <c r="C14" t="s" s="18">
+        <v>56</v>
+      </c>
+      <c r="D14" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E14" t="s" s="16">
+        <v>55</v>
+      </c>
+      <c r="F14" s="17">
+        <v>2938212696</v>
+      </c>
+      <c r="G14" s="19">
+        <v>40939</v>
+      </c>
+      <c r="H14" s="19">
+        <v>40968</v>
+      </c>
+      <c r="I14" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="J14" s="20">
         <v>496310.9</v>
       </c>
+      <c r="K14" t="s" s="16">
+        <v>50</v>
+      </c>
+      <c r="L14" s="17">
+        <v>3621.14</v>
+      </c>
+      <c r="M14" t="s" s="16">
+        <v>51</v>
+      </c>
+      <c r="N14" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="O14" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="P14" s="19">
+        <v>42159</v>
+      </c>
+      <c r="Q14" t="s" s="16">
+        <v>52</v>
+      </c>
+      <c r="R14" t="s" s="16">
+        <v>51</v>
+      </c>
+      <c r="S14" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="T14" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="U14" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="V14" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="W14" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="X14" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="Y14" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="Z14" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AA14" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AB14" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AC14" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AD14" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AE14" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AF14" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AG14" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AH14" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AI14" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AJ14" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AK14" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AL14" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AM14" t="s" s="16">
+        <v>49</v>
+      </c>
     </row>
-    <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="16">
+    <row r="15" ht="30" customHeight="1">
+      <c r="A15" t="s" s="16">
+        <v>45</v>
+      </c>
+      <c r="B15" s="17">
         <v>5766975</v>
       </c>
-      <c r="B11" t="s" s="14">
-        <v>15</v>
-      </c>
-      <c r="C11" t="s" s="15">
-        <v>12</v>
-      </c>
-      <c r="D11" t="s" s="15">
-        <v>12</v>
-      </c>
-      <c r="E11" t="s" s="15">
-        <v>16</v>
-      </c>
-      <c r="F11" s="17">
+      <c r="C15" t="s" s="18">
+        <v>53</v>
+      </c>
+      <c r="D15" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E15" t="s" s="16">
+        <v>48</v>
+      </c>
+      <c r="F15" s="17">
+        <v>2938212691</v>
+      </c>
+      <c r="G15" s="19">
+        <v>40968</v>
+      </c>
+      <c r="H15" s="19">
+        <v>40999</v>
+      </c>
+      <c r="I15" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="J15" s="20">
         <v>1</v>
       </c>
-      <c r="G11" s="17">
+      <c r="K15" t="s" s="16">
+        <v>50</v>
+      </c>
+      <c r="L15" s="17">
+        <v>4915</v>
+      </c>
+      <c r="M15" t="s" s="16">
+        <v>51</v>
+      </c>
+      <c r="N15" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="O15" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="P15" s="19">
+        <v>42159</v>
+      </c>
+      <c r="Q15" t="s" s="16">
+        <v>52</v>
+      </c>
+      <c r="R15" t="s" s="16">
+        <v>51</v>
+      </c>
+      <c r="S15" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="T15" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="U15" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="V15" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="W15" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="X15" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="Y15" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="Z15" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AA15" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AB15" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AC15" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AD15" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AE15" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AF15" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AG15" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AH15" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AI15" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AJ15" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AK15" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AL15" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AM15" t="s" s="16">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" ht="30" customHeight="1">
+      <c r="A16" t="s" s="16">
+        <v>45</v>
+      </c>
+      <c r="B16" s="17">
+        <v>5766975</v>
+      </c>
+      <c r="C16" t="s" s="18">
+        <v>53</v>
+      </c>
+      <c r="D16" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E16" t="s" s="16">
+        <v>48</v>
+      </c>
+      <c r="F16" s="17">
+        <v>2938212692</v>
+      </c>
+      <c r="G16" s="19">
+        <v>40968</v>
+      </c>
+      <c r="H16" s="19">
+        <v>40999</v>
+      </c>
+      <c r="I16" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="J16" s="20">
+        <v>2</v>
+      </c>
+      <c r="K16" t="s" s="16">
+        <v>50</v>
+      </c>
+      <c r="L16" s="17">
+        <v>4180</v>
+      </c>
+      <c r="M16" t="s" s="16">
+        <v>51</v>
+      </c>
+      <c r="N16" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="O16" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="P16" s="19">
+        <v>42159</v>
+      </c>
+      <c r="Q16" t="s" s="16">
+        <v>52</v>
+      </c>
+      <c r="R16" t="s" s="16">
+        <v>51</v>
+      </c>
+      <c r="S16" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="T16" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="U16" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="V16" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="W16" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="X16" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="Y16" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="Z16" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AA16" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AB16" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AC16" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AD16" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AE16" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AF16" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AG16" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AH16" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AI16" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AJ16" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AK16" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AL16" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AM16" t="s" s="16">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" ht="30" customHeight="1">
+      <c r="A17" t="s" s="16">
+        <v>45</v>
+      </c>
+      <c r="B17" s="17">
+        <v>5766975</v>
+      </c>
+      <c r="C17" t="s" s="18">
+        <v>56</v>
+      </c>
+      <c r="D17" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E17" t="s" s="16">
+        <v>55</v>
+      </c>
+      <c r="F17" s="17">
+        <v>2938212695</v>
+      </c>
+      <c r="G17" s="19">
+        <v>40968</v>
+      </c>
+      <c r="H17" s="19">
+        <v>40999</v>
+      </c>
+      <c r="I17" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="J17" s="17">
         <v>1</v>
       </c>
+      <c r="K17" t="s" s="16">
+        <v>50</v>
+      </c>
+      <c r="L17" s="17">
+        <v>4296</v>
+      </c>
+      <c r="M17" t="s" s="16">
+        <v>51</v>
+      </c>
+      <c r="N17" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="O17" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="P17" s="19">
+        <v>42159</v>
+      </c>
+      <c r="Q17" t="s" s="16">
+        <v>52</v>
+      </c>
+      <c r="R17" t="s" s="16">
+        <v>51</v>
+      </c>
+      <c r="S17" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="T17" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="U17" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="V17" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="W17" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="X17" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="Y17" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="Z17" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AA17" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AB17" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AC17" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AD17" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AE17" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AF17" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AG17" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AH17" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AI17" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AJ17" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AK17" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AL17" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AM17" t="s" s="16">
+        <v>49</v>
+      </c>
     </row>
-    <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="16">
+    <row r="18" ht="30" customHeight="1">
+      <c r="A18" t="s" s="16">
+        <v>45</v>
+      </c>
+      <c r="B18" s="17">
         <v>5766975</v>
       </c>
-      <c r="B12" t="s" s="14">
-        <v>15</v>
-      </c>
-      <c r="C12" t="s" s="15">
-        <v>12</v>
-      </c>
-      <c r="D12" t="s" s="15">
-        <v>12</v>
-      </c>
-      <c r="E12" t="s" s="15">
-        <v>16</v>
-      </c>
-      <c r="F12" s="17">
+      <c r="C18" t="s" s="18">
+        <v>56</v>
+      </c>
+      <c r="D18" t="s" s="16">
+        <v>47</v>
+      </c>
+      <c r="E18" t="s" s="16">
+        <v>55</v>
+      </c>
+      <c r="F18" s="17">
+        <v>2938212696</v>
+      </c>
+      <c r="G18" s="19">
+        <v>40968</v>
+      </c>
+      <c r="H18" s="19">
+        <v>40999</v>
+      </c>
+      <c r="I18" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="J18" s="20">
         <v>2</v>
       </c>
-      <c r="G12" s="17">
-        <v>2</v>
+      <c r="K18" t="s" s="16">
+        <v>50</v>
+      </c>
+      <c r="L18" s="17">
+        <v>3621.14</v>
+      </c>
+      <c r="M18" t="s" s="16">
+        <v>51</v>
+      </c>
+      <c r="N18" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="O18" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="P18" s="19">
+        <v>42159</v>
+      </c>
+      <c r="Q18" t="s" s="16">
+        <v>52</v>
+      </c>
+      <c r="R18" t="s" s="16">
+        <v>51</v>
+      </c>
+      <c r="S18" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="T18" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="U18" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="V18" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="W18" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="X18" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="Y18" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="Z18" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AA18" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AB18" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AC18" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AD18" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AE18" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AF18" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AG18" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AH18" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AI18" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AJ18" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AK18" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AL18" t="s" s="16">
+        <v>49</v>
+      </c>
+      <c r="AM18" t="s" s="16">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+  <mergeCells count="3">
+    <mergeCell ref="R5:AD5"/>
+    <mergeCell ref="AE5:AI5"/>
+    <mergeCell ref="AJ5:AM5"/>
   </mergeCells>
-  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="landscape" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Cost can be read from PM Meter imports
</commit_message>
<xml_diff>
--- a/seed/data_importer/tests/data/example-pm-monthly-meter-usage-1-dup.xlsx
+++ b/seed/data_importer/tests/data/example-pm-monthly-meter-usage-1-dup.xlsx
@@ -387,7 +387,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -450,6 +450,9 @@
     </xf>
     <xf numFmtId="59" fontId="5" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1920,8 +1923,8 @@
       <c r="K7" t="s" s="16">
         <v>50</v>
       </c>
-      <c r="L7" s="17">
-        <v>4342</v>
+      <c r="L7" t="s" s="21">
+        <v>49</v>
       </c>
       <c r="M7" t="s" s="16">
         <v>51</v>
@@ -2039,8 +2042,8 @@
       <c r="K8" t="s" s="16">
         <v>50</v>
       </c>
-      <c r="L8" s="17">
-        <v>4975.55</v>
+      <c r="L8" t="s" s="21">
+        <v>49</v>
       </c>
       <c r="M8" t="s" s="16">
         <v>51</v>
@@ -2158,8 +2161,8 @@
       <c r="K9" t="s" s="16">
         <v>50</v>
       </c>
-      <c r="L9" s="17">
-        <v>4915</v>
+      <c r="L9" t="s" s="21">
+        <v>49</v>
       </c>
       <c r="M9" t="s" s="16">
         <v>51</v>
@@ -2277,8 +2280,8 @@
       <c r="K10" t="s" s="16">
         <v>50</v>
       </c>
-      <c r="L10" s="17">
-        <v>4180</v>
+      <c r="L10" t="s" s="21">
+        <v>49</v>
       </c>
       <c r="M10" t="s" s="16">
         <v>51</v>
@@ -2396,8 +2399,8 @@
       <c r="K11" t="s" s="16">
         <v>50</v>
       </c>
-      <c r="L11" s="17">
-        <v>4020.24</v>
+      <c r="L11" t="s" s="21">
+        <v>49</v>
       </c>
       <c r="M11" t="s" s="16">
         <v>51</v>
@@ -2515,8 +2518,8 @@
       <c r="K12" t="s" s="16">
         <v>50</v>
       </c>
-      <c r="L12" s="17">
-        <v>3859.62</v>
+      <c r="L12" t="s" s="21">
+        <v>49</v>
       </c>
       <c r="M12" t="s" s="16">
         <v>51</v>
@@ -2634,8 +2637,8 @@
       <c r="K13" t="s" s="16">
         <v>50</v>
       </c>
-      <c r="L13" s="17">
-        <v>4296</v>
+      <c r="L13" t="s" s="21">
+        <v>49</v>
       </c>
       <c r="M13" t="s" s="16">
         <v>51</v>
@@ -2753,8 +2756,8 @@
       <c r="K14" t="s" s="16">
         <v>50</v>
       </c>
-      <c r="L14" s="17">
-        <v>3621.14</v>
+      <c r="L14" t="s" s="21">
+        <v>49</v>
       </c>
       <c r="M14" t="s" s="16">
         <v>51</v>
@@ -2872,8 +2875,8 @@
       <c r="K15" t="s" s="16">
         <v>50</v>
       </c>
-      <c r="L15" s="17">
-        <v>4915</v>
+      <c r="L15" t="s" s="21">
+        <v>49</v>
       </c>
       <c r="M15" t="s" s="16">
         <v>51</v>
@@ -2991,8 +2994,8 @@
       <c r="K16" t="s" s="16">
         <v>50</v>
       </c>
-      <c r="L16" s="17">
-        <v>4180</v>
+      <c r="L16" t="s" s="21">
+        <v>49</v>
       </c>
       <c r="M16" t="s" s="16">
         <v>51</v>
@@ -3110,8 +3113,8 @@
       <c r="K17" t="s" s="16">
         <v>50</v>
       </c>
-      <c r="L17" s="17">
-        <v>4296</v>
+      <c r="L17" t="s" s="21">
+        <v>49</v>
       </c>
       <c r="M17" t="s" s="16">
         <v>51</v>
@@ -3229,8 +3232,8 @@
       <c r="K18" t="s" s="16">
         <v>50</v>
       </c>
-      <c r="L18" s="17">
-        <v>3621.14</v>
+      <c r="L18" t="s" s="21">
+        <v>49</v>
       </c>
       <c r="M18" t="s" s="16">
         <v>51</v>

</xml_diff>